<commit_message>
change to 6 sats setting
</commit_message>
<xml_diff>
--- a/Satellites/6SatsConstellation.xlsx
+++ b/Satellites/6SatsConstellation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github_Code\Bsk_MARL\Satellites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fanmy019\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964D1EC6-C6B9-480F-88B5-5A5E2FBA7794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B161EB9A-BBC8-4410-A195-67F063C04C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="2145" windowWidth="21600" windowHeight="11333" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -89,13 +89,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -431,17 +431,17 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -481,7 +481,7 @@
         <v>6.9099999999999999E-4</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -510,7 +510,7 @@
         <v>6.9099999999999999E-4</v>
       </c>
       <c r="D3">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -539,7 +539,7 @@
         <v>6.9099999999999999E-4</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>-6</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -568,7 +568,7 @@
         <v>6.9099999999999999E-4</v>
       </c>
       <c r="D5">
-        <v>-4</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -597,7 +597,7 @@
         <v>6.9099999999999999E-4</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>-10</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -626,7 +626,7 @@
         <v>6.9099999999999999E-4</v>
       </c>
       <c r="D7">
-        <v>-6</v>
+        <v>10</v>
       </c>
       <c r="E7">
         <v>0</v>

</xml_diff>